<commit_message>
Performed transformation of means and sds into percentages using min and max values of relevant scale.
</commit_message>
<xml_diff>
--- a/df_appl_v_orange.xlsx
+++ b/df_appl_v_orange.xlsx
@@ -1046,328 +1046,328 @@
     <t xml:space="preserve">smfq</t>
   </si>
   <si>
+    <t xml:space="preserve">Makover, 2019_The High School Transition Program (HSTP)_cau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March, 2004_cbt_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anxiety, disruptive behaviour, obsessive-compulsice/tic, substance use, attention-deficit/hyperactivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March_2004_Fluoxetine_Placebo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RADS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martinovic, 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martinovic, 2006_cbt_cau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moeini, 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAD (Dorehye Amozeshie Dokhtaran)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moeini, 2019_DAD (Dorehye Amozeshie Dokhtaran)_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mufson, 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clinical monitoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mufson, 1999_ipt_clinical monitoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mufson, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mufson, 2004_ipt_cau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mirtazapine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FDA trial - poor reporting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organon_2002a_Mirtazapine_Placebo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organon_2002b_Mirtazapine_Placebo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paxil (GlaxoSmithKline)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paxil (GlaxoSmithKline)_2009_Paroxetine_Placebo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puig-Antich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responder: if K-SADS scores in both depressed mood and anhedonia were ≤2. Non-responder: if K-SADS score for at least one of these two key items were ≥3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puig-Antich_1987_Imipramine_Placebo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reynolds, 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relaxation training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reynolds, 1986_cbt_Relaxation training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reynolds, 1986_cbt_wlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohde, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">life skills/tutoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conduct disorder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohde, 2004_cbt_life skills/tutoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohde, 2014a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cognitive behavioral intervention (CB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">educational brochure control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K-SADS (adapted)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohde, 2014a_cognitive behavioral intervention (CB)_educational brochure control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rossello, 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rossello, 1999_cbt_wlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rossello, 1999_ipt_wlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanford, 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family Psychoeducation (FPE) + cau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanford, 2006_Family Psychoeducation (FPE) + cau_cau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santomauro, 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santomauro, 2016_cbt_wlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shomaker, 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shomaker, 2016_cbt_psychoeducation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Srivastava, 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cCBT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Srivastava, 2020_cCBT_cau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stallard, 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attention control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stallard, 2012_cbt_attention control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stallard, 2012_cbt_cau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stark, 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stark, 1987_pst_wlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">self control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stark, 1987_self control_wlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stice, 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cbt based bibliotherapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessment only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stice, 2008_cbt based bibliotherapy_assessment only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K-SADS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stice, 2008_cbt_assessment only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stice, 2008_sup_assessment only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stikkelbroek, 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stikkelbroek, 2020_cbt_cau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szigethy, 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szigethy, 2007_cbt_cau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tang, 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intensive Interpersonal Psychotherapy for depressed adolescents with suicidal risk (IPT-A-IN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">school-based supportive intervention and psychoeducation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tang, 2009_Intensive Interpersonal Psychotherapy for depressed adolescents with suicidal risk (IPT-A-IN)_school-based supportive intervention and psychoeducation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topooco, 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topooco, 2018_cbt_attention control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phq-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phq_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topooco, 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icbt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimal attention controlÂ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topooco, 2019_icbt_minimal attention controlÂ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Von Knorring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citalopram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European, multi-centered (31 recruitment sites)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Ask Charlotte to check paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Von Knorring_2006_Citalopram_Placebo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K-SADS depression and anhedonia scores ≤2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vostanis, 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non-focused intervention</t>
+  </si>
+  <si>
     <t xml:space="preserve">mfq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Makover, 2019_The High School Transition Program (HSTP)_cau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March, 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March, 2004_cbt_NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anxiety, disruptive behaviour, obsessive-compulsice/tic, substance use, attention-deficit/hyperactivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March_2004_Fluoxetine_Placebo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RADS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martinovic, 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martinovic, 2006_cbt_cau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moeini, 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAD (Dorehye Amozeshie Dokhtaran)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moeini, 2019_DAD (Dorehye Amozeshie Dokhtaran)_NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mufson, 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clinical monitoring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mufson, 1999_ipt_clinical monitoring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mufson, 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mufson, 2004_ipt_cau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mirtazapine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FDA trial - poor reporting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organon_2002a_Mirtazapine_Placebo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organon_2002b_Mirtazapine_Placebo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paxil (GlaxoSmithKline)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paxil (GlaxoSmithKline)_2009_Paroxetine_Placebo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puig-Antich</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Responder: if K-SADS scores in both depressed mood and anhedonia were ≤2. Non-responder: if K-SADS score for at least one of these two key items were ≥3.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puig-Antich_1987_Imipramine_Placebo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reynolds, 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relaxation training</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reynolds, 1986_cbt_Relaxation training</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reynolds, 1986_cbt_wlc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohde, 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">life skills/tutoring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conduct disorder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohde, 2004_cbt_life skills/tutoring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohde, 2014a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cognitive behavioral intervention (CB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">educational brochure control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K-SADS (adapted)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohde, 2014a_cognitive behavioral intervention (CB)_educational brochure control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rossello, 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rossello, 1999_cbt_wlc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rossello, 1999_ipt_wlc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sanford, 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family Psychoeducation (FPE) + cau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">can</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MDD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sanford, 2006_Family Psychoeducation (FPE) + cau_cau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Santomauro, 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Santomauro, 2016_cbt_wlc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shomaker, 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shomaker, 2016_cbt_psychoeducation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Srivastava, 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cCBT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Srivastava, 2020_cCBT_cau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stallard, 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attention control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stallard, 2012_cbt_attention control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stallard, 2012_cbt_cau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stark, 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stark, 1987_pst_wlc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">self control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stark, 1987_self control_wlc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stice, 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cbt based bibliotherapy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessment only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stice, 2008_cbt based bibliotherapy_assessment only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K-SADS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stice, 2008_cbt_assessment only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stice, 2008_sup_assessment only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stikkelbroek, 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stikkelbroek, 2020_cbt_cau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Szigethy, 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Szigethy, 2007_cbt_cau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tang, 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intensive Interpersonal Psychotherapy for depressed adolescents with suicidal risk (IPT-A-IN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">school-based supportive intervention and psychoeducation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tang, 2009_Intensive Interpersonal Psychotherapy for depressed adolescents with suicidal risk (IPT-A-IN)_school-based supportive intervention and psychoeducation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topooco, 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topooco, 2018_cbt_attention control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phq-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phq_9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topooco, 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">icbt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minimal attention controlÂ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topooco, 2019_icbt_minimal attention controlÂ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Von Knorring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Citalopram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">European, multi-centered (31 recruitment sites)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Ask Charlotte to check paper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Von Knorring_2006_Citalopram_Placebo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K-SADS depression and anhedonia scores ≤2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vostanis, 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">non-focused intervention</t>
   </si>
   <si>
     <t xml:space="preserve">Vostanis, 1996_cbt_non-focused intervention</t>
@@ -22103,7 +22103,7 @@
         <v>343</v>
       </c>
       <c r="K107" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L107" t="n">
         <v>7</v>
@@ -22180,7 +22180,7 @@
       <c r="BP107"/>
       <c r="BQ107"/>
       <c r="BR107" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="BS107"/>
       <c r="BT107"/>
@@ -22215,7 +22215,7 @@
         <v>60</v>
       </c>
       <c r="C108" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D108" t="s">
         <v>201</v>
@@ -22334,7 +22334,7 @@
       </c>
       <c r="BQ108"/>
       <c r="BR108" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="BS108"/>
       <c r="BT108"/>
@@ -22371,7 +22371,7 @@
         <v>61</v>
       </c>
       <c r="C109" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D109" t="s">
         <v>201</v>
@@ -22488,7 +22488,7 @@
       </c>
       <c r="BQ109"/>
       <c r="BR109" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="BS109"/>
       <c r="BT109"/>
@@ -22527,7 +22527,7 @@
         <v>56</v>
       </c>
       <c r="C110" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D110" t="s">
         <v>201</v>
@@ -22644,7 +22644,7 @@
         <v>143</v>
       </c>
       <c r="BB110" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BC110" t="s">
         <v>131</v>
@@ -22688,7 +22688,7 @@
         <v>-3.16639477977161</v>
       </c>
       <c r="BR110" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="BS110" t="n">
         <v>-22.64</v>
@@ -22765,7 +22765,7 @@
         <v>57</v>
       </c>
       <c r="C111" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D111" t="s">
         <v>201</v>
@@ -22782,7 +22782,7 @@
       <c r="H111"/>
       <c r="I111"/>
       <c r="J111" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K111" t="s">
         <v>293</v>
@@ -22882,7 +22882,7 @@
         <v>143</v>
       </c>
       <c r="BB111" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BC111" t="s">
         <v>131</v>
@@ -22926,7 +22926,7 @@
         <v>-1.4134755210858</v>
       </c>
       <c r="BR111" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="BS111"/>
       <c r="BT111"/>
@@ -22963,7 +22963,7 @@
         <v>58</v>
       </c>
       <c r="C112" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D112" t="s">
         <v>201</v>
@@ -23050,7 +23050,7 @@
         <v>143</v>
       </c>
       <c r="BB112" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BC112" t="s">
         <v>131</v>
@@ -23082,7 +23082,7 @@
       <c r="BP112"/>
       <c r="BQ112"/>
       <c r="BR112" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="BS112"/>
       <c r="BT112"/>
@@ -23117,7 +23117,7 @@
         <v>62</v>
       </c>
       <c r="C113" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D113" t="s">
         <v>138</v>
@@ -23262,7 +23262,7 @@
         <v>0.0746268656716415</v>
       </c>
       <c r="BR113" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="BS113"/>
       <c r="BT113"/>
@@ -23301,7 +23301,7 @@
         <v>63</v>
       </c>
       <c r="C114" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D114" t="s">
         <v>138</v>
@@ -23442,7 +23442,7 @@
         <v>-0.165745856353591</v>
       </c>
       <c r="BR114" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="BS114"/>
       <c r="BT114"/>
@@ -23481,7 +23481,7 @@
         <v>64</v>
       </c>
       <c r="C115" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D115" t="s">
         <v>138</v>
@@ -23622,7 +23622,7 @@
         <v>-0.0655737704918034</v>
       </c>
       <c r="BR115" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="BS115"/>
       <c r="BT115"/>
@@ -23661,7 +23661,7 @@
         <v>65</v>
       </c>
       <c r="C116" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D116" t="s">
         <v>253</v>
@@ -23676,7 +23676,7 @@
         <v>1</v>
       </c>
       <c r="H116" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I116"/>
       <c r="J116" t="s">
@@ -23804,7 +23804,7 @@
         <v>-0.0656934306569345</v>
       </c>
       <c r="BR116" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="BS116"/>
       <c r="BT116"/>
@@ -23843,7 +23843,7 @@
         <v>66</v>
       </c>
       <c r="C117" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D117" t="s">
         <v>189</v>
@@ -23861,7 +23861,7 @@
         <v>158</v>
       </c>
       <c r="I117" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J117" t="s">
         <v>101</v>
@@ -23988,7 +23988,7 @@
         <v>-0.788571428571428</v>
       </c>
       <c r="BR117" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="BS117"/>
       <c r="BT117"/>
@@ -24027,7 +24027,7 @@
         <v>67</v>
       </c>
       <c r="C118" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D118" t="s">
         <v>189</v>
@@ -24045,7 +24045,7 @@
         <v>158</v>
       </c>
       <c r="I118" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J118" t="s">
         <v>149</v>
@@ -24168,7 +24168,7 @@
         <v>-0.853448275862069</v>
       </c>
       <c r="BR118" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="BS118"/>
       <c r="BT118"/>
@@ -24207,7 +24207,7 @@
         <v>68</v>
       </c>
       <c r="C119" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D119" t="s">
         <v>201</v>
@@ -24352,7 +24352,7 @@
         <v>-0.82089552238806</v>
       </c>
       <c r="BR119" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="BS119"/>
       <c r="BT119"/>
@@ -24391,7 +24391,7 @@
         <v>69</v>
       </c>
       <c r="C120" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D120" t="s">
         <v>201</v>
@@ -24532,7 +24532,7 @@
         <v>-1.04395604395604</v>
       </c>
       <c r="BR120" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="BS120"/>
       <c r="BT120"/>
@@ -24573,13 +24573,13 @@
         <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D121" t="s">
         <v>167</v>
       </c>
       <c r="E121" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F121" t="s">
         <v>127</v>
@@ -24698,7 +24698,7 @@
         <v>133</v>
       </c>
       <c r="BL121" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="BM121"/>
       <c r="BN121" t="n">
@@ -24714,7 +24714,7 @@
         <v>-1.42686550108559</v>
       </c>
       <c r="BR121" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="BS121" t="n">
         <v>-15.85</v>
@@ -24783,13 +24783,13 @@
         <v>2</v>
       </c>
       <c r="C122" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D122" t="s">
         <v>174</v>
       </c>
       <c r="E122" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F122" t="s">
         <v>127</v>
@@ -24922,7 +24922,7 @@
         <v>-0.855730773625871</v>
       </c>
       <c r="BR122" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="BS122" t="n">
         <v>-13.48</v>
@@ -24991,7 +24991,7 @@
         <v>59</v>
       </c>
       <c r="C123" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D123" t="s">
         <v>114</v>
@@ -25093,7 +25093,7 @@
       </c>
       <c r="BB123"/>
       <c r="BC123" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="BD123" t="s">
         <v>132</v>
@@ -25130,7 +25130,7 @@
       <c r="BP123"/>
       <c r="BQ123"/>
       <c r="BR123" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="BS123" t="n">
         <v>-16.5</v>
@@ -25215,7 +25215,7 @@
         <v>60</v>
       </c>
       <c r="C124" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D124" t="s">
         <v>114</v>
@@ -25303,7 +25303,7 @@
       </c>
       <c r="BB124"/>
       <c r="BC124" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="BD124" t="s">
         <v>132</v>
@@ -25332,7 +25332,7 @@
       <c r="BP124"/>
       <c r="BQ124"/>
       <c r="BR124" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="BS124"/>
       <c r="BT124"/>
@@ -25369,10 +25369,10 @@
         <v>61</v>
       </c>
       <c r="C125" t="s">
+        <v>369</v>
+      </c>
+      <c r="D125" t="s">
         <v>370</v>
-      </c>
-      <c r="D125" t="s">
-        <v>371</v>
       </c>
       <c r="E125" t="s">
         <v>281</v>
@@ -25440,7 +25440,7 @@
       <c r="AD125"/>
       <c r="AE125"/>
       <c r="AF125" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AG125" t="n">
         <v>9</v>
@@ -25542,7 +25542,7 @@
         <v>-1.44736842105263</v>
       </c>
       <c r="BR125" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="BS125" t="n">
         <v>-1.2</v>
@@ -25617,10 +25617,10 @@
         <v>73</v>
       </c>
       <c r="C126" t="s">
+        <v>373</v>
+      </c>
+      <c r="D126" t="s">
         <v>374</v>
-      </c>
-      <c r="D126" t="s">
-        <v>375</v>
       </c>
       <c r="E126" t="s">
         <v>98</v>
@@ -25635,7 +25635,7 @@
         <v>98</v>
       </c>
       <c r="I126" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J126" t="s">
         <v>149</v>
@@ -25758,7 +25758,7 @@
         <v>-2.18532818532819</v>
       </c>
       <c r="BR126" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="BS126"/>
       <c r="BT126"/>
@@ -25797,10 +25797,10 @@
         <v>75</v>
       </c>
       <c r="C127" t="s">
+        <v>373</v>
+      </c>
+      <c r="D127" t="s">
         <v>374</v>
-      </c>
-      <c r="D127" t="s">
-        <v>375</v>
       </c>
       <c r="E127" t="s">
         <v>98</v>
@@ -25815,7 +25815,7 @@
         <v>98</v>
       </c>
       <c r="I127" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J127" t="s">
         <v>293</v>
@@ -25938,7 +25938,7 @@
         <v>-1.73107207752877</v>
       </c>
       <c r="BR127" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="BS127"/>
       <c r="BT127"/>
@@ -25977,10 +25977,10 @@
         <v>74</v>
       </c>
       <c r="C128" t="s">
+        <v>373</v>
+      </c>
+      <c r="D128" t="s">
         <v>374</v>
-      </c>
-      <c r="D128" t="s">
-        <v>375</v>
       </c>
       <c r="E128" t="s">
         <v>98</v>
@@ -25995,7 +25995,7 @@
         <v>98</v>
       </c>
       <c r="I128" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J128" t="s">
         <v>294</v>
@@ -26118,7 +26118,7 @@
         <v>-1.65606668724915</v>
       </c>
       <c r="BR128" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="BS128"/>
       <c r="BT128"/>
@@ -26157,10 +26157,10 @@
         <v>70</v>
       </c>
       <c r="C129" t="s">
+        <v>373</v>
+      </c>
+      <c r="D129" t="s">
         <v>374</v>
-      </c>
-      <c r="D129" t="s">
-        <v>375</v>
       </c>
       <c r="E129" t="s">
         <v>98</v>
@@ -26302,7 +26302,7 @@
         <v>0.184313725490196</v>
       </c>
       <c r="BR129" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="BS129"/>
       <c r="BT129"/>
@@ -26341,10 +26341,10 @@
         <v>72</v>
       </c>
       <c r="C130" t="s">
+        <v>373</v>
+      </c>
+      <c r="D130" t="s">
         <v>374</v>
-      </c>
-      <c r="D130" t="s">
-        <v>375</v>
       </c>
       <c r="E130" t="s">
         <v>98</v>
@@ -26482,7 +26482,7 @@
         <v>0.0492957746478875</v>
       </c>
       <c r="BR130" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="BS130"/>
       <c r="BT130"/>
@@ -26521,10 +26521,10 @@
         <v>71</v>
       </c>
       <c r="C131" t="s">
+        <v>373</v>
+      </c>
+      <c r="D131" t="s">
         <v>374</v>
-      </c>
-      <c r="D131" t="s">
-        <v>375</v>
       </c>
       <c r="E131" t="s">
         <v>98</v>
@@ -26662,7 +26662,7 @@
         <v>1.14944237918216</v>
       </c>
       <c r="BR131" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="BS131"/>
       <c r="BT131"/>
@@ -26701,7 +26701,7 @@
         <v>77</v>
       </c>
       <c r="C132" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D132" t="s">
         <v>201</v>
@@ -26719,7 +26719,7 @@
         <v>98</v>
       </c>
       <c r="I132" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J132" t="s">
         <v>101</v>
@@ -26837,7 +26837,7 @@
       </c>
       <c r="BL132"/>
       <c r="BM132" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="BN132"/>
       <c r="BO132"/>
@@ -26848,7 +26848,7 @@
         <v>0.393162393162393</v>
       </c>
       <c r="BR132" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="BS132"/>
       <c r="BT132"/>
@@ -26887,7 +26887,7 @@
         <v>76</v>
       </c>
       <c r="C133" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D133" t="s">
         <v>201</v>
@@ -26905,7 +26905,7 @@
         <v>98</v>
       </c>
       <c r="I133" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J133" t="s">
         <v>149</v>
@@ -27019,7 +27019,7 @@
       </c>
       <c r="BL133"/>
       <c r="BM133" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="BN133"/>
       <c r="BO133"/>
@@ -27030,7 +27030,7 @@
         <v>0.174311926605505</v>
       </c>
       <c r="BR133" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="BS133"/>
       <c r="BT133"/>
@@ -27069,7 +27069,7 @@
         <v>118</v>
       </c>
       <c r="C134" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D134" t="s">
         <v>125</v>
@@ -27084,13 +27084,13 @@
         <v>1</v>
       </c>
       <c r="H134" t="s">
+        <v>383</v>
+      </c>
+      <c r="I134" t="s">
         <v>384</v>
       </c>
-      <c r="I134" t="s">
+      <c r="J134" t="s">
         <v>385</v>
-      </c>
-      <c r="J134" t="s">
-        <v>386</v>
       </c>
       <c r="K134" t="s">
         <v>152</v>
@@ -27210,7 +27210,7 @@
         <v>0.311688311688312</v>
       </c>
       <c r="BR134" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="BS134"/>
       <c r="BT134"/>
@@ -27249,7 +27249,7 @@
         <v>78</v>
       </c>
       <c r="C135" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D135" t="s">
         <v>189</v>
@@ -27394,7 +27394,7 @@
         <v>-0.670826833073323</v>
       </c>
       <c r="BR135" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="BS135"/>
       <c r="BT135"/>
@@ -27433,7 +27433,7 @@
         <v>79</v>
       </c>
       <c r="C136" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D136" t="s">
         <v>189</v>
@@ -27578,7 +27578,7 @@
         <v>-0.670826833073323</v>
       </c>
       <c r="BR136" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="BS136"/>
       <c r="BT136"/>
@@ -27617,7 +27617,7 @@
         <v>80</v>
       </c>
       <c r="C137" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D137" t="s">
         <v>138</v>
@@ -27632,7 +27632,7 @@
         <v>1</v>
       </c>
       <c r="H137" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I137" t="s">
         <v>115</v>
@@ -27703,7 +27703,7 @@
       </c>
       <c r="BB137"/>
       <c r="BC137" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="BD137"/>
       <c r="BE137" t="n">
@@ -27717,7 +27717,7 @@
       <c r="BI137"/>
       <c r="BJ137"/>
       <c r="BK137" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="BL137"/>
       <c r="BM137"/>
@@ -27726,7 +27726,7 @@
       <c r="BP137"/>
       <c r="BQ137"/>
       <c r="BR137" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="BS137"/>
       <c r="BT137"/>
@@ -27761,7 +27761,7 @@
         <v>81</v>
       </c>
       <c r="C138" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D138" t="s">
         <v>177</v>
@@ -27782,10 +27782,10 @@
         <v>100</v>
       </c>
       <c r="J138" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K138" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="L138" t="n">
         <v>99</v>
@@ -27897,7 +27897,7 @@
       </c>
       <c r="BL138"/>
       <c r="BM138" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="BN138"/>
       <c r="BO138"/>
@@ -27908,7 +27908,7 @@
         <v>0.20610349402919</v>
       </c>
       <c r="BR138" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="BS138"/>
       <c r="BT138"/>
@@ -27947,7 +27947,7 @@
         <v>84</v>
       </c>
       <c r="C139" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D139" t="s">
         <v>177</v>
@@ -28076,7 +28076,7 @@
         <v>-1.42666666666667</v>
       </c>
       <c r="BR139" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="BS139"/>
       <c r="BT139"/>
@@ -28115,7 +28115,7 @@
         <v>86</v>
       </c>
       <c r="C140" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D140" t="s">
         <v>204</v>
@@ -28130,7 +28130,7 @@
         <v>1</v>
       </c>
       <c r="H140" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I140" t="s">
         <v>115</v>
@@ -28256,7 +28256,7 @@
         <v>-3.29770992366412</v>
       </c>
       <c r="BR140" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="BS140"/>
       <c r="BT140"/>
@@ -28295,7 +28295,7 @@
         <v>85</v>
       </c>
       <c r="C141" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D141" t="s">
         <v>204</v>
@@ -28310,7 +28310,7 @@
         <v>1</v>
       </c>
       <c r="H141" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I141" t="s">
         <v>115</v>
@@ -28436,7 +28436,7 @@
         <v>-1.77319587628866</v>
       </c>
       <c r="BR141" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="BS141"/>
       <c r="BT141"/>
@@ -28475,7 +28475,7 @@
         <v>87</v>
       </c>
       <c r="C142" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D142" t="s">
         <v>334</v>
@@ -28493,13 +28493,13 @@
         <v>98</v>
       </c>
       <c r="I142" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J142" t="s">
         <v>343</v>
       </c>
       <c r="K142" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L142" t="n">
         <v>7</v>
@@ -28589,7 +28589,7 @@
       </c>
       <c r="BB142"/>
       <c r="BC142" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="BD142"/>
       <c r="BE142" t="n">
@@ -28616,7 +28616,7 @@
         <v>-0.398104265402843</v>
       </c>
       <c r="BR142" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="BS142"/>
       <c r="BT142"/>
@@ -28655,7 +28655,7 @@
         <v>88</v>
       </c>
       <c r="C143" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D143" t="s">
         <v>334</v>
@@ -28679,7 +28679,7 @@
         <v>343</v>
       </c>
       <c r="K143" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L143" t="n">
         <v>7</v>
@@ -28773,7 +28773,7 @@
       </c>
       <c r="BB143"/>
       <c r="BC143" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="BD143"/>
       <c r="BE143" t="n">
@@ -28800,7 +28800,7 @@
         <v>-0.705550329256821</v>
       </c>
       <c r="BR143" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="BS143"/>
       <c r="BT143"/>
@@ -28839,13 +28839,13 @@
         <v>91</v>
       </c>
       <c r="C144" t="s">
+        <v>409</v>
+      </c>
+      <c r="D144" t="s">
+        <v>370</v>
+      </c>
+      <c r="E144" t="s">
         <v>410</v>
-      </c>
-      <c r="D144" t="s">
-        <v>371</v>
-      </c>
-      <c r="E144" t="s">
-        <v>411</v>
       </c>
       <c r="F144" t="s">
         <v>99</v>
@@ -28854,7 +28854,7 @@
         <v>1</v>
       </c>
       <c r="H144" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I144" t="s">
         <v>100</v>
@@ -28984,7 +28984,7 @@
         <v>-0.349079263410729</v>
       </c>
       <c r="BR144" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="BS144"/>
       <c r="BT144"/>
@@ -29023,13 +29023,13 @@
         <v>89</v>
       </c>
       <c r="C145" t="s">
+        <v>409</v>
+      </c>
+      <c r="D145" t="s">
+        <v>370</v>
+      </c>
+      <c r="E145" t="s">
         <v>410</v>
-      </c>
-      <c r="D145" t="s">
-        <v>371</v>
-      </c>
-      <c r="E145" t="s">
-        <v>411</v>
       </c>
       <c r="F145" t="s">
         <v>99</v>
@@ -29038,7 +29038,7 @@
         <v>1</v>
       </c>
       <c r="H145" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I145" t="s">
         <v>100</v>
@@ -29164,7 +29164,7 @@
         <v>-0.152602324406266</v>
       </c>
       <c r="BR145" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="BS145"/>
       <c r="BT145"/>
@@ -29203,13 +29203,13 @@
         <v>90</v>
       </c>
       <c r="C146" t="s">
+        <v>409</v>
+      </c>
+      <c r="D146" t="s">
+        <v>370</v>
+      </c>
+      <c r="E146" t="s">
         <v>410</v>
-      </c>
-      <c r="D146" t="s">
-        <v>371</v>
-      </c>
-      <c r="E146" t="s">
-        <v>411</v>
       </c>
       <c r="F146" t="s">
         <v>99</v>
@@ -29218,16 +29218,16 @@
         <v>1</v>
       </c>
       <c r="H146" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I146" t="s">
         <v>100</v>
       </c>
       <c r="J146" t="s">
+        <v>412</v>
+      </c>
+      <c r="K146" t="s">
         <v>413</v>
-      </c>
-      <c r="K146" t="s">
-        <v>414</v>
       </c>
       <c r="L146" t="n">
         <v>10</v>
@@ -29344,7 +29344,7 @@
         <v>-0.374746597161888</v>
       </c>
       <c r="BR146" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="BS146"/>
       <c r="BT146"/>
@@ -29383,13 +29383,13 @@
         <v>92</v>
       </c>
       <c r="C147" t="s">
+        <v>409</v>
+      </c>
+      <c r="D147" t="s">
+        <v>370</v>
+      </c>
+      <c r="E147" t="s">
         <v>410</v>
-      </c>
-      <c r="D147" t="s">
-        <v>371</v>
-      </c>
-      <c r="E147" t="s">
-        <v>411</v>
       </c>
       <c r="F147" t="s">
         <v>99</v>
@@ -29398,7 +29398,7 @@
         <v>1</v>
       </c>
       <c r="H147" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I147" t="s">
         <v>100</v>
@@ -29524,7 +29524,7 @@
         <v>0.322781988408382</v>
       </c>
       <c r="BR147" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="BS147"/>
       <c r="BT147"/>
@@ -29563,10 +29563,10 @@
         <v>95</v>
       </c>
       <c r="C148" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D148" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E148" t="s">
         <v>208</v>
@@ -29578,7 +29578,7 @@
         <v>1</v>
       </c>
       <c r="H148" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I148" t="s">
         <v>100</v>
@@ -29708,7 +29708,7 @@
         <v>-0.349079263410729</v>
       </c>
       <c r="BR148" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="BS148"/>
       <c r="BT148"/>
@@ -29747,10 +29747,10 @@
         <v>93</v>
       </c>
       <c r="C149" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D149" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E149" t="s">
         <v>208</v>
@@ -29762,7 +29762,7 @@
         <v>1</v>
       </c>
       <c r="H149" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I149" t="s">
         <v>100</v>
@@ -29888,7 +29888,7 @@
         <v>-0.152602324406266</v>
       </c>
       <c r="BR149" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="BS149"/>
       <c r="BT149"/>
@@ -29927,10 +29927,10 @@
         <v>94</v>
       </c>
       <c r="C150" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D150" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E150" t="s">
         <v>208</v>
@@ -29942,16 +29942,16 @@
         <v>1</v>
       </c>
       <c r="H150" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I150" t="s">
         <v>100</v>
       </c>
       <c r="J150" t="s">
+        <v>412</v>
+      </c>
+      <c r="K150" t="s">
         <v>413</v>
-      </c>
-      <c r="K150" t="s">
-        <v>414</v>
       </c>
       <c r="L150" t="n">
         <v>10</v>
@@ -30068,7 +30068,7 @@
         <v>-0.374746597161888</v>
       </c>
       <c r="BR150" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="BS150"/>
       <c r="BT150"/>
@@ -30107,10 +30107,10 @@
         <v>96</v>
       </c>
       <c r="C151" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D151" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E151" t="s">
         <v>208</v>
@@ -30122,7 +30122,7 @@
         <v>1</v>
       </c>
       <c r="H151" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I151" t="s">
         <v>100</v>
@@ -30248,7 +30248,7 @@
         <v>0.322781988408382</v>
       </c>
       <c r="BR151" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="BS151"/>
       <c r="BT151"/>
@@ -30287,10 +30287,10 @@
         <v>99</v>
       </c>
       <c r="C152" t="s">
+        <v>416</v>
+      </c>
+      <c r="D152" t="s">
         <v>417</v>
-      </c>
-      <c r="D152" t="s">
-        <v>418</v>
       </c>
       <c r="E152" t="s">
         <v>98</v>
@@ -30302,10 +30302,10 @@
         <v>1</v>
       </c>
       <c r="H152" t="s">
+        <v>418</v>
+      </c>
+      <c r="I152" t="s">
         <v>419</v>
-      </c>
-      <c r="I152" t="s">
-        <v>420</v>
       </c>
       <c r="J152" t="s">
         <v>149</v>
@@ -30428,7 +30428,7 @@
         <v>-0.304691618344755</v>
       </c>
       <c r="BR152" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="BS152"/>
       <c r="BT152"/>
@@ -30467,10 +30467,10 @@
         <v>100</v>
       </c>
       <c r="C153" t="s">
+        <v>416</v>
+      </c>
+      <c r="D153" t="s">
         <v>417</v>
-      </c>
-      <c r="D153" t="s">
-        <v>418</v>
       </c>
       <c r="E153" t="s">
         <v>98</v>
@@ -30482,13 +30482,13 @@
         <v>1</v>
       </c>
       <c r="H153" t="s">
+        <v>418</v>
+      </c>
+      <c r="I153" t="s">
         <v>419</v>
       </c>
-      <c r="I153" t="s">
-        <v>420</v>
-      </c>
       <c r="J153" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K153" t="s">
         <v>152</v>
@@ -30608,7 +30608,7 @@
         <v>-0.303030303030303</v>
       </c>
       <c r="BR153" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="BS153"/>
       <c r="BT153"/>
@@ -30647,10 +30647,10 @@
         <v>97</v>
       </c>
       <c r="C154" t="s">
+        <v>416</v>
+      </c>
+      <c r="D154" t="s">
         <v>417</v>
-      </c>
-      <c r="D154" t="s">
-        <v>418</v>
       </c>
       <c r="E154" t="s">
         <v>98</v>
@@ -30665,7 +30665,7 @@
         <v>98</v>
       </c>
       <c r="I154" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J154" t="s">
         <v>149</v>
@@ -30792,7 +30792,7 @@
         <v>-0.304691618344755</v>
       </c>
       <c r="BR154" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="BS154"/>
       <c r="BT154"/>
@@ -30831,10 +30831,10 @@
         <v>98</v>
       </c>
       <c r="C155" t="s">
+        <v>416</v>
+      </c>
+      <c r="D155" t="s">
         <v>417</v>
-      </c>
-      <c r="D155" t="s">
-        <v>418</v>
       </c>
       <c r="E155" t="s">
         <v>98</v>
@@ -30849,10 +30849,10 @@
         <v>98</v>
       </c>
       <c r="I155" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J155" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K155" t="s">
         <v>152</v>
@@ -30972,7 +30972,7 @@
         <v>-0.303030303030303</v>
       </c>
       <c r="BR155" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="BS155"/>
       <c r="BT155"/>
@@ -31011,13 +31011,13 @@
         <v>101</v>
       </c>
       <c r="C156" t="s">
+        <v>416</v>
+      </c>
+      <c r="D156" t="s">
         <v>417</v>
       </c>
-      <c r="D156" t="s">
-        <v>418</v>
-      </c>
       <c r="E156" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F156" t="s">
         <v>115</v>
@@ -31026,10 +31026,10 @@
         <v>1</v>
       </c>
       <c r="H156" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I156" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J156" t="s">
         <v>149</v>
@@ -31156,7 +31156,7 @@
         <v>-0.304691618344755</v>
       </c>
       <c r="BR156" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="BS156"/>
       <c r="BT156"/>
@@ -31195,13 +31195,13 @@
         <v>102</v>
       </c>
       <c r="C157" t="s">
+        <v>416</v>
+      </c>
+      <c r="D157" t="s">
         <v>417</v>
       </c>
-      <c r="D157" t="s">
-        <v>418</v>
-      </c>
       <c r="E157" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F157" t="s">
         <v>115</v>
@@ -31210,13 +31210,13 @@
         <v>1</v>
       </c>
       <c r="H157" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I157" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J157" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K157" t="s">
         <v>152</v>
@@ -31336,7 +31336,7 @@
         <v>-0.303030303030303</v>
       </c>
       <c r="BR157" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="BS157"/>
       <c r="BT157"/>
@@ -31375,7 +31375,7 @@
         <v>103</v>
       </c>
       <c r="C158" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D158" t="s">
         <v>204</v>
@@ -31396,7 +31396,7 @@
         <v>115</v>
       </c>
       <c r="J158" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K158" t="s">
         <v>152</v>
@@ -31476,7 +31476,7 @@
       <c r="BP158"/>
       <c r="BQ158"/>
       <c r="BR158" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="BS158"/>
       <c r="BT158"/>
@@ -31511,7 +31511,7 @@
         <v>104</v>
       </c>
       <c r="C159" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D159" t="s">
         <v>157</v>
@@ -31656,7 +31656,7 @@
         <v>-0.53125</v>
       </c>
       <c r="BR159" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="BS159"/>
       <c r="BT159"/>
@@ -31695,7 +31695,7 @@
         <v>105</v>
       </c>
       <c r="C160" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D160" t="s">
         <v>157</v>
@@ -31716,7 +31716,7 @@
         <v>115</v>
       </c>
       <c r="J160" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K160" t="s">
         <v>152</v>
@@ -31836,7 +31836,7 @@
         <v>0.0571428571428572</v>
       </c>
       <c r="BR160" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="BS160"/>
       <c r="BT160"/>
@@ -31875,7 +31875,7 @@
         <v>120</v>
       </c>
       <c r="C161" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D161" t="s">
         <v>114</v>
@@ -31890,10 +31890,10 @@
         <v>1</v>
       </c>
       <c r="H161" t="s">
+        <v>430</v>
+      </c>
+      <c r="I161" t="s">
         <v>431</v>
-      </c>
-      <c r="I161" t="s">
-        <v>432</v>
       </c>
       <c r="J161" t="s">
         <v>215</v>
@@ -31989,7 +31989,7 @@
       </c>
       <c r="BB161"/>
       <c r="BC161" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="BD161"/>
       <c r="BE161" t="n">
@@ -32018,7 +32018,7 @@
         <v>-0.0714630613230325</v>
       </c>
       <c r="BR161" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="BS161"/>
       <c r="BT161"/>
@@ -32057,10 +32057,10 @@
         <v>121</v>
       </c>
       <c r="C162" t="s">
+        <v>434</v>
+      </c>
+      <c r="D162" t="s">
         <v>435</v>
-      </c>
-      <c r="D162" t="s">
-        <v>436</v>
       </c>
       <c r="E162" t="s">
         <v>98</v>
@@ -32075,7 +32075,7 @@
         <v>98</v>
       </c>
       <c r="I162" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J162" t="s">
         <v>215</v>
@@ -32202,7 +32202,7 @@
         <v>-0.788888888888889</v>
       </c>
       <c r="BR162" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="BS162"/>
       <c r="BT162"/>
@@ -32241,10 +32241,10 @@
         <v>122</v>
       </c>
       <c r="C163" t="s">
+        <v>434</v>
+      </c>
+      <c r="D163" t="s">
         <v>435</v>
-      </c>
-      <c r="D163" t="s">
-        <v>436</v>
       </c>
       <c r="E163" t="s">
         <v>98</v>
@@ -32259,13 +32259,13 @@
         <v>98</v>
       </c>
       <c r="I163" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J163" t="s">
+        <v>437</v>
+      </c>
+      <c r="K163" t="s">
         <v>438</v>
-      </c>
-      <c r="K163" t="s">
-        <v>439</v>
       </c>
       <c r="L163" t="n">
         <v>99</v>
@@ -32382,7 +32382,7 @@
         <v>-1.025</v>
       </c>
       <c r="BR163" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="BS163"/>
       <c r="BT163"/>
@@ -32421,7 +32421,7 @@
         <v>106</v>
       </c>
       <c r="C164" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D164" t="s">
         <v>253</v>
@@ -32436,10 +32436,10 @@
         <v>1</v>
       </c>
       <c r="H164" t="s">
+        <v>440</v>
+      </c>
+      <c r="I164" t="s">
         <v>441</v>
-      </c>
-      <c r="I164" t="s">
-        <v>442</v>
       </c>
       <c r="J164" t="s">
         <v>149</v>
@@ -32562,7 +32562,7 @@
         <v>-0.437158469945355</v>
       </c>
       <c r="BR164" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="BS164"/>
       <c r="BT164"/>
@@ -32603,13 +32603,13 @@
         <v>63</v>
       </c>
       <c r="C165" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D165" t="s">
         <v>138</v>
       </c>
       <c r="E165" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F165" t="s">
         <v>127</v>
@@ -32707,7 +32707,7 @@
       </c>
       <c r="BB165"/>
       <c r="BC165" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="BD165" t="s">
         <v>306</v>
@@ -32728,7 +32728,7 @@
         <v>133</v>
       </c>
       <c r="BL165" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="BM165"/>
       <c r="BN165" t="n">
@@ -32742,7 +32742,7 @@
         <v>-2.16545454545455</v>
       </c>
       <c r="BR165" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="BS165" t="n">
         <v>-12.09</v>
@@ -32827,13 +32827,13 @@
         <v>62</v>
       </c>
       <c r="C166" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D166" t="s">
         <v>138</v>
       </c>
       <c r="E166" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F166" t="s">
         <v>127</v>
@@ -32894,7 +32894,7 @@
       <c r="AD166"/>
       <c r="AE166"/>
       <c r="AF166" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="AG166"/>
       <c r="AH166"/>
@@ -32927,7 +32927,7 @@
       </c>
       <c r="BB166"/>
       <c r="BC166" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="BD166" t="s">
         <v>306</v>
@@ -32956,7 +32956,7 @@
       <c r="BP166"/>
       <c r="BQ166"/>
       <c r="BR166" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="BS166"/>
       <c r="BT166"/>
@@ -32991,7 +32991,7 @@
         <v>107</v>
       </c>
       <c r="C167" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D167" t="s">
         <v>315</v>
@@ -33009,13 +33009,13 @@
         <v>98</v>
       </c>
       <c r="I167" t="s">
+        <v>450</v>
+      </c>
+      <c r="J167" t="s">
         <v>451</v>
       </c>
-      <c r="J167" t="s">
-        <v>344</v>
-      </c>
       <c r="K167" t="s">
-        <v>344</v>
+        <v>451</v>
       </c>
       <c r="L167" t="n">
         <v>7</v>
@@ -33105,7 +33105,7 @@
       </c>
       <c r="BB167"/>
       <c r="BC167" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="BD167"/>
       <c r="BE167" t="n">
@@ -33171,7 +33171,7 @@
         <v>108</v>
       </c>
       <c r="C168" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D168" t="s">
         <v>315</v>
@@ -33189,13 +33189,13 @@
         <v>98</v>
       </c>
       <c r="I168" t="s">
+        <v>450</v>
+      </c>
+      <c r="J168" t="s">
         <v>451</v>
       </c>
-      <c r="J168" t="s">
-        <v>344</v>
-      </c>
       <c r="K168" t="s">
-        <v>344</v>
+        <v>451</v>
       </c>
       <c r="L168" t="n">
         <v>7</v>
@@ -33289,7 +33289,7 @@
       </c>
       <c r="BB168"/>
       <c r="BC168" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="BD168"/>
       <c r="BE168" t="n">
@@ -33703,7 +33703,7 @@
         <v>201</v>
       </c>
       <c r="E171" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F171" t="s">
         <v>127</v>
@@ -33939,7 +33939,7 @@
         <v>201</v>
       </c>
       <c r="E172" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F172" t="s">
         <v>127</v>
@@ -35228,10 +35228,10 @@
         <v>474</v>
       </c>
       <c r="J179" t="s">
-        <v>344</v>
+        <v>451</v>
       </c>
       <c r="K179" t="s">
-        <v>344</v>
+        <v>451</v>
       </c>
       <c r="L179" t="n">
         <v>7</v>
@@ -35321,7 +35321,7 @@
       </c>
       <c r="BB179"/>
       <c r="BC179" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="BD179"/>
       <c r="BE179" t="n">
@@ -36153,7 +36153,7 @@
       </c>
       <c r="BB184"/>
       <c r="BC184" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="BD184"/>
       <c r="BE184" t="n">

</xml_diff>